<commit_message>
fixed mitigation for risk bad performance
</commit_message>
<xml_diff>
--- a/risk management/Risk management.xlsx
+++ b/risk management/Risk management.xlsx
@@ -157,13 +157,13 @@
     <t xml:space="preserve">Bad performance of new function</t>
   </si>
   <si>
-    <t xml:space="preserve">Test the new functions by either unit-testing or debugging.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Function not working according to the specification.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modify the function according to the specification, get help from team members.</t>
+    <t xml:space="preserve">Test the new functions for performance (on multiple devices) before publishing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Performance drop after changes, lag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dont release new feature that causes problems, investigate where performance lags, find alternative, faster implementation possibilities</t>
   </si>
   <si>
     <t xml:space="preserve">Natural disasters</t>
@@ -417,17 +417,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:N1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15"/>

</xml_diff>